<commit_message>
B2C.B2B checkout steps update
</commit_message>
<xml_diff>
--- a/resources/testData/GuestCheckout.xlsx
+++ b/resources/testData/GuestCheckout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="5775" tabRatio="526" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -12,7 +12,7 @@
     <sheet name="Settings" sheetId="4" state="hidden" r:id="rId3"/>
     <sheet name="Instructions to Use" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1010,7 +1010,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1843,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79239AFF-C243-4B19-B3C8-902634CC01ED}">
           <x14:formula1>
             <xm:f>Settings!$B:$B</xm:f>

</xml_diff>